<commit_message>
Update files with title of paper as submitted
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_acyl_prop_ranges.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_acyl_prop_ranges.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/LOBSTAHS/inst/doc/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="37200" yWindow="460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C-DB ranges for in silico sim" sheetId="5" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Provided under an Apache 2.0 license; attribution required</t>
   </si>
@@ -92,6 +97,9 @@
   </si>
   <si>
     <t>Navigate to the worksheet "C-DB ranges for in silico sim," then export as a .csv with the filename "LOBSTAHS_acyl_prop_ranges.csv"; this file can be sourced by specifying the file path in the LOBSTAHS database generation function</t>
+  </si>
+  <si>
+    <t>See Collins, J.R., B.R. Edwards, H.F. Fredricks, and B.A.S. Van Mooy, 2016, "LOBSTAHS: A Novel Lipidomics Strategy for Semi-Untargeted Discovery and Identification of Oxidative Stress Biomarkers"</t>
   </si>
 </sst>
 </file>
@@ -569,13 +577,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1">
+    <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>21</v>
@@ -588,7 +596,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1">
+    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -617,7 +625,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -628,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>7</v>
       </c>
@@ -639,7 +647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>8</v>
       </c>
@@ -650,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>9</v>
       </c>
@@ -661,7 +669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>10</v>
       </c>
@@ -678,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>11</v>
       </c>
@@ -695,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>12</v>
       </c>
@@ -712,7 +720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>13</v>
       </c>
@@ -723,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>14</v>
       </c>
@@ -734,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>15</v>
       </c>
@@ -745,7 +753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>16</v>
       </c>
@@ -756,7 +764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>17</v>
       </c>
@@ -767,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>18</v>
       </c>
@@ -778,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>19</v>
       </c>
@@ -789,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>20</v>
       </c>
@@ -806,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>21</v>
       </c>
@@ -823,7 +831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>22</v>
       </c>
@@ -840,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>23</v>
       </c>
@@ -857,7 +865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>24</v>
       </c>
@@ -874,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>25</v>
       </c>
@@ -891,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>26</v>
       </c>
@@ -908,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>27</v>
       </c>
@@ -919,7 +927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>28</v>
       </c>
@@ -930,7 +938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>29</v>
       </c>
@@ -941,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -958,7 +966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>31</v>
       </c>
@@ -975,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>32</v>
       </c>
@@ -992,7 +1000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>33</v>
       </c>
@@ -1009,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>34</v>
       </c>
@@ -1026,7 +1034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>35</v>
       </c>
@@ -1043,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>36</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>37</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>38</v>
       </c>
@@ -1094,7 +1102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>39</v>
       </c>
@@ -1111,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>40</v>
       </c>
@@ -1128,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>41</v>
       </c>
@@ -1145,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>42</v>
       </c>
@@ -1162,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43</v>
       </c>
@@ -1179,7 +1187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44</v>
       </c>
@@ -1196,7 +1204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>46</v>
       </c>
@@ -1230,7 +1238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>47</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>48</v>
       </c>
@@ -1264,7 +1272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>49</v>
       </c>
@@ -1281,7 +1289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>50</v>
       </c>
@@ -1298,7 +1306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>51</v>
       </c>
@@ -1315,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>52</v>
       </c>
@@ -1332,7 +1340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>53</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>54</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>55</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>56</v>
       </c>
@@ -1376,7 +1384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>57</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>58</v>
       </c>
@@ -1398,7 +1406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>59</v>
       </c>
@@ -1409,7 +1417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>60</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>61</v>
       </c>
@@ -1431,7 +1439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>62</v>
       </c>
@@ -1442,7 +1450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>63</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>64</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>65</v>
       </c>
@@ -1475,7 +1483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>66</v>
       </c>
@@ -1486,7 +1494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>67</v>
       </c>
@@ -1497,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>68</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>69</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>70</v>
       </c>
@@ -1530,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>71</v>
       </c>
@@ -1541,7 +1549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>72</v>
       </c>
@@ -1552,7 +1560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>73</v>
       </c>
@@ -1563,7 +1571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>74</v>
       </c>
@@ -1574,7 +1582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>75</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>76</v>
       </c>
@@ -1596,7 +1604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>77</v>
       </c>
@@ -1607,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>78</v>
       </c>
@@ -1624,108 +1632,103 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>42328</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>42344</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit new Excel files for database generation that include IP_MAG and one IP_MAG species class, LPC
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_acyl_prop_ranges.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_acyl_prop_ranges.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37200" yWindow="460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C-DB ranges for in silico sim" sheetId="5" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Provided under an Apache 2.0 license; attribution required</t>
   </si>
@@ -100,6 +103,15 @@
   </si>
   <si>
     <t>See Collins, J.R., B.R. Edwards, H.F. Fredricks, and B.A.S. Van Mooy, 2016, "LOBSTAHS: A Novel Lipidomics Strategy for Semi-Untargeted Discovery and Identification of Oxidative Stress Biomarkers"</t>
+  </si>
+  <si>
+    <t>IP_MAG_min</t>
+  </si>
+  <si>
+    <t>IP_MAG_max</t>
+  </si>
+  <si>
+    <t>Added columns for IP_MAG_min, IP_MAG_max</t>
   </si>
 </sst>
 </file>
@@ -571,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +595,7 @@
     <col min="2" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>21</v>
@@ -595,8 +607,10 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -607,69 +621,75 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>6</v>
       </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>7</v>
       </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>8</v>
       </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>9</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>10</v>
       </c>
@@ -685,8 +705,14 @@
       <c r="G7" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>11</v>
       </c>
@@ -700,10 +726,16 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>12</v>
       </c>
@@ -717,10 +749,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>13</v>
       </c>
@@ -730,8 +768,14 @@
       <c r="E10" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>14</v>
       </c>
@@ -741,8 +785,14 @@
       <c r="E11" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>15</v>
       </c>
@@ -752,8 +802,14 @@
       <c r="E12" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>16</v>
       </c>
@@ -763,8 +819,14 @@
       <c r="E13" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>17</v>
       </c>
@@ -774,8 +836,14 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>18</v>
       </c>
@@ -785,8 +853,14 @@
       <c r="E15" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>19</v>
       </c>
@@ -796,8 +870,14 @@
       <c r="E16" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>20</v>
       </c>
@@ -813,8 +893,14 @@
       <c r="E17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>21</v>
       </c>
@@ -830,8 +916,14 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>22</v>
       </c>
@@ -847,8 +939,14 @@
       <c r="E19" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>23</v>
       </c>
@@ -864,8 +962,14 @@
       <c r="E20" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>24</v>
       </c>
@@ -881,8 +985,14 @@
       <c r="E21" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>25</v>
       </c>
@@ -898,8 +1008,14 @@
       <c r="E22" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>26</v>
       </c>
@@ -915,8 +1031,14 @@
       <c r="E23" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>27</v>
       </c>
@@ -927,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>28</v>
       </c>
@@ -938,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>29</v>
       </c>
@@ -949,7 +1071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -959,14 +1081,14 @@
       <c r="C27" s="3">
         <v>7</v>
       </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>31</v>
       </c>
@@ -976,14 +1098,14 @@
       <c r="C28" s="3">
         <v>7</v>
       </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>32</v>
       </c>
@@ -993,14 +1115,14 @@
       <c r="C29" s="3">
         <v>8</v>
       </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>33</v>
       </c>
@@ -1010,14 +1132,14 @@
       <c r="C30" s="3">
         <v>8</v>
       </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>34</v>
       </c>
@@ -1027,14 +1149,14 @@
       <c r="C31" s="3">
         <v>9</v>
       </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>35</v>
       </c>
@@ -1044,14 +1166,14 @@
       <c r="C32" s="3">
         <v>8</v>
       </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>36</v>
       </c>
@@ -1061,14 +1183,14 @@
       <c r="C33" s="3">
         <v>10</v>
       </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>37</v>
       </c>
@@ -1078,14 +1200,14 @@
       <c r="C34" s="3">
         <v>8</v>
       </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>38</v>
       </c>
@@ -1095,14 +1217,14 @@
       <c r="C35" s="3">
         <v>10</v>
       </c>
-      <c r="H35" s="3">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>39</v>
       </c>
@@ -1112,14 +1234,14 @@
       <c r="C36" s="3">
         <v>8</v>
       </c>
-      <c r="H36" s="3">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>40</v>
       </c>
@@ -1129,14 +1251,14 @@
       <c r="C37" s="3">
         <v>11</v>
       </c>
-      <c r="H37" s="3">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>41</v>
       </c>
@@ -1146,14 +1268,14 @@
       <c r="C38" s="3">
         <v>8</v>
       </c>
-      <c r="H38" s="3">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>42</v>
       </c>
@@ -1163,14 +1285,14 @@
       <c r="C39" s="3">
         <v>11</v>
       </c>
-      <c r="H39" s="3">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43</v>
       </c>
@@ -1180,14 +1302,14 @@
       <c r="C40" s="3">
         <v>8</v>
       </c>
-      <c r="H40" s="3">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44</v>
       </c>
@@ -1197,14 +1319,14 @@
       <c r="C41" s="3">
         <v>12</v>
       </c>
-      <c r="H41" s="3">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45</v>
       </c>
@@ -1214,14 +1336,14 @@
       <c r="C42" s="3">
         <v>8</v>
       </c>
-      <c r="H42" s="3">
-        <v>0</v>
-      </c>
-      <c r="I42" s="3">
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>46</v>
       </c>
@@ -1231,14 +1353,14 @@
       <c r="C43" s="3">
         <v>8</v>
       </c>
-      <c r="H43" s="3">
-        <v>0</v>
-      </c>
-      <c r="I43" s="3">
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>47</v>
       </c>
@@ -1248,14 +1370,14 @@
       <c r="C44" s="3">
         <v>8</v>
       </c>
-      <c r="H44" s="3">
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>48</v>
       </c>
@@ -1265,14 +1387,14 @@
       <c r="C45" s="3">
         <v>8</v>
       </c>
-      <c r="H45" s="3">
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>49</v>
       </c>
@@ -1282,14 +1404,14 @@
       <c r="C46" s="3">
         <v>4</v>
       </c>
-      <c r="H46" s="3">
-        <v>0</v>
-      </c>
-      <c r="I46" s="3">
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>50</v>
       </c>
@@ -1299,14 +1421,14 @@
       <c r="C47" s="3">
         <v>4</v>
       </c>
-      <c r="H47" s="3">
-        <v>0</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>51</v>
       </c>
@@ -1316,14 +1438,14 @@
       <c r="C48" s="3">
         <v>4</v>
       </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
-      <c r="I48" s="3">
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>52</v>
       </c>
@@ -1333,302 +1455,302 @@
       <c r="C49" s="3">
         <v>4</v>
       </c>
-      <c r="H49" s="3">
-        <v>0</v>
-      </c>
-      <c r="I49" s="3">
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>53</v>
       </c>
-      <c r="H50" s="3">
-        <v>0</v>
-      </c>
-      <c r="I50" s="3">
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>54</v>
       </c>
-      <c r="H51" s="3">
-        <v>0</v>
-      </c>
-      <c r="I51" s="3">
+      <c r="J51" s="3">
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>55</v>
       </c>
-      <c r="H52" s="3">
-        <v>0</v>
-      </c>
-      <c r="I52" s="3">
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>56</v>
       </c>
-      <c r="H53" s="3">
-        <v>0</v>
-      </c>
-      <c r="I53" s="3">
+      <c r="J53" s="3">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>57</v>
       </c>
-      <c r="H54" s="3">
-        <v>0</v>
-      </c>
-      <c r="I54" s="3">
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>58</v>
       </c>
-      <c r="H55" s="3">
-        <v>0</v>
-      </c>
-      <c r="I55" s="3">
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>59</v>
       </c>
-      <c r="H56" s="3">
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>60</v>
       </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="3">
+      <c r="J57" s="3">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>61</v>
       </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>62</v>
       </c>
-      <c r="H59" s="3">
-        <v>0</v>
-      </c>
-      <c r="I59" s="3">
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>63</v>
       </c>
-      <c r="H60" s="3">
-        <v>0</v>
-      </c>
-      <c r="I60" s="3">
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>64</v>
       </c>
-      <c r="H61" s="3">
-        <v>0</v>
-      </c>
-      <c r="I61" s="3">
+      <c r="J61" s="3">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>65</v>
       </c>
-      <c r="H62" s="3">
-        <v>0</v>
-      </c>
-      <c r="I62" s="3">
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>66</v>
       </c>
-      <c r="H63" s="3">
-        <v>0</v>
-      </c>
-      <c r="I63" s="3">
+      <c r="J63" s="3">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>67</v>
       </c>
-      <c r="H64" s="3">
-        <v>0</v>
-      </c>
-      <c r="I64" s="3">
+      <c r="J64" s="3">
+        <v>0</v>
+      </c>
+      <c r="K64" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>68</v>
       </c>
-      <c r="H65" s="3">
-        <v>0</v>
-      </c>
-      <c r="I65" s="3">
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>69</v>
       </c>
-      <c r="H66" s="3">
-        <v>0</v>
-      </c>
-      <c r="I66" s="3">
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>70</v>
       </c>
-      <c r="H67" s="3">
-        <v>0</v>
-      </c>
-      <c r="I67" s="3">
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>71</v>
       </c>
-      <c r="H68" s="3">
-        <v>0</v>
-      </c>
-      <c r="I68" s="3">
+      <c r="J68" s="3">
+        <v>0</v>
+      </c>
+      <c r="K68" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>72</v>
       </c>
-      <c r="H69" s="3">
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
+      <c r="J69" s="3">
+        <v>0</v>
+      </c>
+      <c r="K69" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>73</v>
       </c>
-      <c r="H70" s="3">
-        <v>0</v>
-      </c>
-      <c r="I70" s="3">
+      <c r="J70" s="3">
+        <v>0</v>
+      </c>
+      <c r="K70" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>74</v>
       </c>
-      <c r="H71" s="3">
-        <v>0</v>
-      </c>
-      <c r="I71" s="3">
+      <c r="J71" s="3">
+        <v>0</v>
+      </c>
+      <c r="K71" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>75</v>
       </c>
-      <c r="H72" s="3">
-        <v>0</v>
-      </c>
-      <c r="I72" s="3">
+      <c r="J72" s="3">
+        <v>0</v>
+      </c>
+      <c r="K72" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>76</v>
       </c>
-      <c r="H73" s="3">
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
+      <c r="J73" s="3">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>77</v>
       </c>
-      <c r="H74" s="3">
-        <v>0</v>
-      </c>
-      <c r="I74" s="3">
+      <c r="J74" s="3">
+        <v>0</v>
+      </c>
+      <c r="K74" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>78</v>
       </c>
-      <c r="H75" s="3">
-        <v>0</v>
-      </c>
-      <c r="I75" s="3">
+      <c r="J75" s="3">
+        <v>0</v>
+      </c>
+      <c r="K75" s="3">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1637,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1727,6 +1849,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>42607</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>